<commit_message>
Fix a few cells that were mislabelled
</commit_message>
<xml_diff>
--- a/lfp_atn_simuran/cell_lists/CTRL_Lesion_cells_filled.xlsx
+++ b/lfp_atn_simuran/cell_lists/CTRL_Lesion_cells_filled.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SubRet_recordings_imaging\SIMURAN\cell_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repos\lfp_atn\lfp_atn_simuran\cell_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87082BE3-BF5A-4431-95D8-11B50EA44037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D0E920-3273-4E5D-9063-F4E93B37E97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2554,7 +2554,7 @@
         <v>3</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H64" t="s">
         <v>19</v>
@@ -2902,7 +2902,7 @@
         <v>4</v>
       </c>
       <c r="G76">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H76" t="s">
         <v>29</v>
@@ -2931,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="G77">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H77" t="s">
         <v>29</v>
@@ -3047,7 +3047,7 @@
         <v>2</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H81" t="s">
         <v>19</v>
@@ -3076,7 +3076,7 @@
         <v>2</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H82" t="s">
         <v>19</v>
@@ -3482,7 +3482,7 @@
         <v>4</v>
       </c>
       <c r="G96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H96" t="s">
         <v>38</v>
@@ -3511,7 +3511,7 @@
         <v>3</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H97" t="s">
         <v>19</v>

</xml_diff>